<commit_message>
Aggiunta la Tabella con le medie dei valori per ogni specie
</commit_message>
<xml_diff>
--- a/docs/Punti_INFC_rilievi.xlsx
+++ b/docs/Punti_INFC_rilievi.xlsx
@@ -4,14 +4,28 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="180" windowWidth="3150" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="6456" yWindow="180" windowWidth="3156" windowHeight="7092" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PUNTI" sheetId="1" r:id="rId1"/>
     <sheet name="LEGENDA" sheetId="2" r:id="rId2"/>
     <sheet name="ALBERI" sheetId="3" r:id="rId3"/>
+    <sheet name="Medie_per_specie" sheetId="6" r:id="rId4"/>
+    <sheet name="Foglio1" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="input278849" localSheetId="4">Foglio1!$C$14:$U$17</definedName>
+    <definedName name="input280026" localSheetId="4">Foglio1!$D$13:$V$14</definedName>
+    <definedName name="input281673" localSheetId="4">Foglio1!$G$5:$W$12</definedName>
+    <definedName name="input282422" localSheetId="4">Foglio1!$G$12:$W$12</definedName>
+    <definedName name="input282679" localSheetId="4">Foglio1!$B$13:$T$16</definedName>
+    <definedName name="input282921" localSheetId="4">Foglio1!$D$13:$V$14</definedName>
+    <definedName name="input282928" localSheetId="4">Foglio1!$G$1:$W$2</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId6"/>
+  </pivotCaches>
 </workbook>
 </file>
 
@@ -50,8 +64,167 @@
 </comments>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="input278849" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alessandro Scremin\Documents\PROGETTI\ForSE\testData\corineLandCover\input278849.txt" comma="1">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="input280026" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alessandro Scremin\Documents\PROGETTI\ForSE\testData\corineLandCover\input280026.txt" comma="1">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="input281673" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alessandro Scremin\Documents\PROGETTI\ForSE\testData\corineLandCover\input281673.txt" comma="1">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="input282422" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alessandro Scremin\Documents\PROGETTI\ForSE\testData\corineLandCover\input282422.txt" comma="1">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="input282679" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alessandro Scremin\Documents\PROGETTI\ForSE\testData\corineLandCover\input282679.txt" comma="1">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="input282921" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alessandro Scremin\Documents\PROGETTI\ForSE\testData\corineLandCover\input282921.txt" comma="1">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="input282928" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alessandro Scremin\Documents\PROGETTI\ForSE\testData\corineLandCover\input282928.txt" comma="1">
+      <textFields count="16">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="214">
   <si>
     <t>IDPUNTO</t>
   </si>
@@ -594,12 +767,115 @@
   </si>
   <si>
     <t>06_2006</t>
+  </si>
+  <si>
+    <t>Fagussylvatica</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Phenology</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Lai</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Stool</t>
+  </si>
+  <si>
+    <t>AvDBH</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Wf</t>
+  </si>
+  <si>
+    <t>Wrc</t>
+  </si>
+  <si>
+    <t>Wrf</t>
+  </si>
+  <si>
+    <t>Ws</t>
+  </si>
+  <si>
+    <t>Wres</t>
+  </si>
+  <si>
+    <t>quercus_deciduous</t>
+  </si>
+  <si>
+    <t>quercus_evergreen</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Castaneasativa</t>
+  </si>
+  <si>
+    <t>Copertura Landcover</t>
+  </si>
+  <si>
+    <t>2 e 7</t>
+  </si>
+  <si>
+    <t>1 e 6 e 7</t>
+  </si>
+  <si>
+    <t>Valori</t>
+  </si>
+  <si>
+    <t>Media di Age</t>
+  </si>
+  <si>
+    <t>Media di N</t>
+  </si>
+  <si>
+    <t>Media di AvDBH</t>
+  </si>
+  <si>
+    <t>Media di Height</t>
+  </si>
+  <si>
+    <t>Etichette di riga</t>
+  </si>
+  <si>
+    <t>Totale complessivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.00000000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -667,7 +943,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,6 +953,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,7 +993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -731,11 +1031,167 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="44">
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -743,6 +1199,514 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Alessandro Scremin" refreshedDate="41243.712199884256" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="10">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:R11" sheet="Foglio1"/>
+  </cacheSource>
+  <cacheFields count="18">
+    <cacheField name="IDPUNTO" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="278849" maxValue="282928"/>
+    </cacheField>
+    <cacheField name="ANNO RIL" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="LAT_ND_W84" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="37.844516519999999" maxValue="37.989339999999999"/>
+    </cacheField>
+    <cacheField name="LON_ND_W84" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="14.04271855" maxValue="14.193776"/>
+    </cacheField>
+    <cacheField name="NORD_ND_GB" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4188925" maxValue="4204946"/>
+    </cacheField>
+    <cacheField name="EST_ND_GB" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2435773" maxValue="2449209"/>
+    </cacheField>
+    <cacheField name="x" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="y" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="Age" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="100"/>
+    </cacheField>
+    <cacheField name="Species" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Fagussylvatica"/>
+        <s v="quercus_deciduous"/>
+        <s v="quercus_evergreen"/>
+        <s v="Castaneasativa"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Copertura Landcover" numFmtId="0">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="7"/>
+    </cacheField>
+    <cacheField name="Phenology" numFmtId="0">
+      <sharedItems count="2">
+        <s v="D"/>
+        <s v="E"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Management" numFmtId="0">
+      <sharedItems count="1">
+        <s v="T"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Lai" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="N" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="130"/>
+    </cacheField>
+    <cacheField name="Stool" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="AvDBH" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="5" maxValue="34.58"/>
+    </cacheField>
+    <cacheField name="Height" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.8" maxValue="15.97"/>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
+  <r>
+    <n v="282928"/>
+    <s v="09_2006"/>
+    <n v="37.844516519999999"/>
+    <n v="14.12224812"/>
+    <n v="4188925"/>
+    <n v="2442771"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="100"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="34.58"/>
+    <n v="15.97"/>
+  </r>
+  <r>
+    <n v="281673"/>
+    <s v="11_2006"/>
+    <n v="37.889564020000002"/>
+    <n v="14.055055449999999"/>
+    <n v="4193981"/>
+    <n v="2436909"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="10"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="7"/>
+    <n v="0"/>
+    <n v="31.37"/>
+    <n v="10.33"/>
+  </r>
+  <r>
+    <n v="281673"/>
+    <s v="11_2006"/>
+    <n v="37.889564020000002"/>
+    <n v="14.055055449999999"/>
+    <n v="4193981"/>
+    <n v="2436909"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="10"/>
+    <x v="1"/>
+    <n v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="12"/>
+    <n v="0"/>
+    <n v="14.7"/>
+    <n v="9.1199999999999992"/>
+  </r>
+  <r>
+    <n v="282422"/>
+    <s v="09_2006"/>
+    <n v="37.862535559999998"/>
+    <n v="14.05446987"/>
+    <n v="4190983"/>
+    <n v="2436827"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="23"/>
+    <n v="0"/>
+    <n v="17.46"/>
+    <n v="9.1999999999999993"/>
+  </r>
+  <r>
+    <n v="282422"/>
+    <s v="09_2006"/>
+    <n v="37.862535559999998"/>
+    <n v="14.05446987"/>
+    <n v="4190983"/>
+    <n v="2436827"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="2"/>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="15.17"/>
+    <n v="9.06"/>
+  </r>
+  <r>
+    <n v="282921"/>
+    <s v="10_2006"/>
+    <n v="37.844516519999999"/>
+    <n v="14.04271855"/>
+    <n v="4188994"/>
+    <n v="2435773"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="20"/>
+    <x v="0"/>
+    <s v="2 e 7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="130"/>
+    <n v="0"/>
+    <n v="14.14"/>
+    <n v="10.98"/>
+  </r>
+  <r>
+    <n v="280026"/>
+    <s v="10_2006"/>
+    <n v="37.943620559999999"/>
+    <n v="14.14724182"/>
+    <n v="4199901"/>
+    <n v="2445070"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="20"/>
+    <x v="2"/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="20"/>
+    <n v="0"/>
+    <n v="7.5"/>
+    <n v="4.18"/>
+  </r>
+  <r>
+    <n v="280026"/>
+    <s v="10_2006"/>
+    <n v="37.943620559999999"/>
+    <n v="14.14724182"/>
+    <n v="4199901"/>
+    <n v="2445070"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="20"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="2.8"/>
+  </r>
+  <r>
+    <n v="278849"/>
+    <s v="03_2009"/>
+    <n v="37.989339999999999"/>
+    <n v="14.193776"/>
+    <n v="4204946"/>
+    <n v="2449209"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="2"/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="7"/>
+    <n v="0"/>
+    <n v="32.75"/>
+    <n v="7.76"/>
+  </r>
+  <r>
+    <n v="282679"/>
+    <s v="09_2006"/>
+    <n v="37.853526049999999"/>
+    <n v="14.14517684"/>
+    <n v="4189906"/>
+    <n v="2444797"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="25"/>
+    <x v="3"/>
+    <s v="1 e 6 e 7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="18.329999999999998"/>
+    <n v="12.79"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:E17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="9"/>
+    <field x="11"/>
+    <field x="12"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="Media di AvDBH" fld="16" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Media di Height" fld="17" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Media di Age" fld="8" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Media di N" fld="14" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="8">
+    <format dxfId="36">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="37">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="9" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="11" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="40">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="41">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="11" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="43">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="9" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="11" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="input282679" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="input278849" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="input280026" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="input282921" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="input282422" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="input281673" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="input282928" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1034,20 +1998,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1">
@@ -1409,8 +2373,12 @@
       <c r="B10" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="5">
+        <v>37.989339999999999</v>
+      </c>
+      <c r="D10" s="5">
+        <v>14.193776</v>
+      </c>
       <c r="E10" s="18">
         <v>4204946</v>
       </c>
@@ -1485,328 +2453,328 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="522" max="522" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="523" max="523" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="778" max="778" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="779" max="779" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="1034" max="1034" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1035" max="1035" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="1290" max="1290" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1291" max="1291" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="1546" max="1546" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1547" max="1547" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="1802" max="1802" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="1803" max="1803" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2058" max="2058" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2059" max="2059" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2314" max="2314" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2315" max="2315" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2570" max="2570" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2571" max="2571" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2826" max="2826" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2827" max="2827" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3082" max="3082" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3083" max="3083" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3338" max="3338" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3339" max="3339" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3594" max="3594" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3595" max="3595" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3850" max="3850" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3851" max="3851" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4106" max="4106" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4107" max="4107" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4362" max="4362" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4363" max="4363" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4618" max="4618" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4619" max="4619" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4874" max="4874" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4875" max="4875" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5130" max="5130" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5131" max="5131" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5386" max="5386" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5387" max="5387" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5642" max="5642" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5643" max="5643" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5898" max="5898" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5899" max="5899" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6154" max="6154" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6155" max="6155" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6410" max="6410" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6411" max="6411" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6666" max="6666" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6667" max="6667" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6922" max="6922" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6923" max="6923" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7178" max="7178" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7179" max="7179" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7434" max="7434" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7435" max="7435" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7690" max="7690" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7691" max="7691" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7946" max="7946" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7947" max="7947" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8202" max="8202" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8203" max="8203" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8458" max="8458" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8459" max="8459" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8714" max="8714" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8715" max="8715" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8970" max="8970" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8971" max="8971" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9226" max="9226" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9227" max="9227" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9482" max="9482" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9483" max="9483" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9738" max="9738" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9739" max="9739" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9994" max="9994" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9995" max="9995" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10250" max="10250" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10251" max="10251" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10506" max="10506" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10507" max="10507" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10762" max="10762" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10763" max="10763" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11018" max="11018" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11019" max="11019" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11274" max="11274" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11275" max="11275" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11530" max="11530" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11531" max="11531" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11786" max="11786" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11787" max="11787" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12042" max="12042" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12043" max="12043" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12298" max="12298" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12299" max="12299" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12554" max="12554" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12555" max="12555" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12810" max="12810" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12811" max="12811" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13066" max="13066" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13067" max="13067" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13322" max="13322" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13323" max="13323" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13578" max="13578" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13579" max="13579" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13834" max="13834" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13835" max="13835" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14090" max="14090" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14091" max="14091" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14346" max="14346" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14347" max="14347" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14602" max="14602" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14603" max="14603" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14858" max="14858" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14859" max="14859" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15114" max="15114" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15115" max="15115" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15370" max="15370" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15371" max="15371" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15626" max="15626" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15627" max="15627" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15882" max="15882" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15883" max="15883" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16138" max="16138" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16139" max="16139" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="522" max="522" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="523" max="523" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="778" max="778" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="779" max="779" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1034" max="1034" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1035" max="1035" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1290" max="1290" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1291" max="1291" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1546" max="1546" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1547" max="1547" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1802" max="1802" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1803" max="1803" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2058" max="2058" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2059" max="2059" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2314" max="2314" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2315" max="2315" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2570" max="2570" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2571" max="2571" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2826" max="2826" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2827" max="2827" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3082" max="3082" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3083" max="3083" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3338" max="3338" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3339" max="3339" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3594" max="3594" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3595" max="3595" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3850" max="3850" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3851" max="3851" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4106" max="4106" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4107" max="4107" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4362" max="4362" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4363" max="4363" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4618" max="4618" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4619" max="4619" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4874" max="4874" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4875" max="4875" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5130" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5131" max="5131" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5386" max="5386" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5387" max="5387" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5642" max="5642" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5643" max="5643" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5898" max="5898" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5899" max="5899" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6154" max="6154" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6155" max="6155" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6410" max="6410" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6411" max="6411" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6666" max="6666" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6667" max="6667" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6922" max="6922" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6923" max="6923" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7178" max="7178" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7179" max="7179" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7434" max="7434" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7435" max="7435" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7690" max="7690" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7691" max="7691" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7946" max="7946" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7947" max="7947" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8202" max="8202" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8203" max="8203" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8458" max="8458" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8459" max="8459" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8714" max="8714" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8715" max="8715" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8970" max="8970" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8971" max="8971" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9226" max="9226" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9227" max="9227" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9482" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9483" max="9483" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9738" max="9738" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9739" max="9739" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9994" max="9994" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9995" max="9995" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10250" max="10250" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10251" max="10251" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10506" max="10506" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10507" max="10507" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10762" max="10762" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10763" max="10763" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11018" max="11018" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11019" max="11019" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11274" max="11274" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11275" max="11275" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11530" max="11530" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11531" max="11531" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11786" max="11786" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11787" max="11787" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12042" max="12042" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12043" max="12043" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12298" max="12298" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12299" max="12299" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12554" max="12554" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12555" max="12555" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12810" max="12810" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12811" max="12811" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13066" max="13066" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13067" max="13067" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13322" max="13322" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13323" max="13323" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13578" max="13578" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13579" max="13579" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13834" max="13834" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13835" max="13835" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14090" max="14090" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14091" max="14091" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14346" max="14346" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14347" max="14347" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14602" max="14602" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14603" max="14603" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14858" max="14858" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="14859" max="14859" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15114" max="15114" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15115" max="15115" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15370" max="15370" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15371" max="15371" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15626" max="15626" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15627" max="15627" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15882" max="15882" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15883" max="15883" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16138" max="16138" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16139" max="16139" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2226,19 +3194,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -6934,4 +7902,1081 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5">
+      <c r="B3" s="24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="29">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C5" s="29">
+        <v>12.79</v>
+      </c>
+      <c r="D5" s="29">
+        <v>25</v>
+      </c>
+      <c r="E5" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="29">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C6" s="29">
+        <v>12.79</v>
+      </c>
+      <c r="D6" s="29">
+        <v>25</v>
+      </c>
+      <c r="E6" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="25">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C7" s="25">
+        <v>12.79</v>
+      </c>
+      <c r="D7" s="25">
+        <v>25</v>
+      </c>
+      <c r="E7" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="29">
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C8" s="29">
+        <v>12.426666666666668</v>
+      </c>
+      <c r="D8" s="29">
+        <v>43.333333333333336</v>
+      </c>
+      <c r="E8" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="29">
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C9" s="29">
+        <v>12.426666666666668</v>
+      </c>
+      <c r="D9" s="29">
+        <v>43.333333333333336</v>
+      </c>
+      <c r="E9" s="29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="25">
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C10" s="25">
+        <v>12.426666666666668</v>
+      </c>
+      <c r="D10" s="25">
+        <v>43.333333333333336</v>
+      </c>
+      <c r="E10" s="25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="29">
+        <v>12.386666666666665</v>
+      </c>
+      <c r="C11" s="29">
+        <v>7.04</v>
+      </c>
+      <c r="D11" s="29">
+        <v>10</v>
+      </c>
+      <c r="E11" s="29">
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="29">
+        <v>12.386666666666665</v>
+      </c>
+      <c r="C12" s="29">
+        <v>7.04</v>
+      </c>
+      <c r="D12" s="29">
+        <v>10</v>
+      </c>
+      <c r="E12" s="29">
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="25">
+        <v>12.386666666666665</v>
+      </c>
+      <c r="C13" s="25">
+        <v>7.04</v>
+      </c>
+      <c r="D13" s="25">
+        <v>10</v>
+      </c>
+      <c r="E13" s="25">
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="29">
+        <v>18.473333333333333</v>
+      </c>
+      <c r="C14" s="29">
+        <v>7</v>
+      </c>
+      <c r="D14" s="29">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E14" s="29">
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="29">
+        <v>18.473333333333333</v>
+      </c>
+      <c r="C15" s="29">
+        <v>7</v>
+      </c>
+      <c r="D15" s="29">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E15" s="29">
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="25">
+        <v>18.473333333333333</v>
+      </c>
+      <c r="C16" s="25">
+        <v>7</v>
+      </c>
+      <c r="D16" s="25">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E16" s="25">
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="25">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C17" s="25">
+        <v>9.2189999999999976</v>
+      </c>
+      <c r="D17" s="25">
+        <v>20.5</v>
+      </c>
+      <c r="E17" s="25">
+        <v>22.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="8" width="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" t="s">
+        <v>191</v>
+      </c>
+      <c r="P1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>193</v>
+      </c>
+      <c r="R1" t="s">
+        <v>194</v>
+      </c>
+      <c r="S1" t="s">
+        <v>195</v>
+      </c>
+      <c r="T1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U1" t="s">
+        <v>197</v>
+      </c>
+      <c r="V1" t="s">
+        <v>198</v>
+      </c>
+      <c r="W1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="11">
+        <v>282928</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="12">
+        <v>37.844516519999999</v>
+      </c>
+      <c r="D2" s="12">
+        <v>14.12224812</v>
+      </c>
+      <c r="E2" s="12">
+        <v>4188925</v>
+      </c>
+      <c r="F2" s="12">
+        <v>2442771</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K2" s="20">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M2" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>34.58</v>
+      </c>
+      <c r="R2">
+        <v>15.97</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="21">
+        <v>281673</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="12">
+        <v>37.889564020000002</v>
+      </c>
+      <c r="D3" s="12">
+        <v>14.055055449999999</v>
+      </c>
+      <c r="E3" s="12">
+        <v>4193981</v>
+      </c>
+      <c r="F3" s="12">
+        <v>2436909</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K3" s="20">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>7</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>31.37</v>
+      </c>
+      <c r="R3">
+        <v>10.33</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="21">
+        <v>281673</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="12">
+        <v>37.889564020000002</v>
+      </c>
+      <c r="D4" s="12">
+        <v>14.055055449999999</v>
+      </c>
+      <c r="E4" s="12">
+        <v>4193981</v>
+      </c>
+      <c r="F4" s="12">
+        <v>2436909</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" s="20">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>182</v>
+      </c>
+      <c r="M4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>14.7</v>
+      </c>
+      <c r="R4">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="22">
+        <v>282422</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="12">
+        <v>37.862535559999998</v>
+      </c>
+      <c r="D5" s="12">
+        <v>14.05446987</v>
+      </c>
+      <c r="E5" s="12">
+        <v>4190983</v>
+      </c>
+      <c r="F5" s="12">
+        <v>2436827</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="K5" s="20">
+        <v>6</v>
+      </c>
+      <c r="L5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>23</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>17.46</v>
+      </c>
+      <c r="R5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" s="22">
+        <v>282422</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="12">
+        <v>37.862535559999998</v>
+      </c>
+      <c r="D6" s="12">
+        <v>14.05446987</v>
+      </c>
+      <c r="E6" s="12">
+        <v>4190983</v>
+      </c>
+      <c r="F6" s="12">
+        <v>2436827</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" s="20">
+        <v>7</v>
+      </c>
+      <c r="L6" t="s">
+        <v>202</v>
+      </c>
+      <c r="M6" t="s">
+        <v>183</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>15.17</v>
+      </c>
+      <c r="R6">
+        <v>9.06</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="11">
+        <v>282921</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="12">
+        <v>37.844516519999999</v>
+      </c>
+      <c r="D7" s="12">
+        <v>14.04271855</v>
+      </c>
+      <c r="E7" s="12">
+        <v>4188994</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2435773</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="L7" t="s">
+        <v>182</v>
+      </c>
+      <c r="M7" t="s">
+        <v>183</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>130</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>14.14</v>
+      </c>
+      <c r="R7">
+        <v>10.98</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="23">
+        <v>280026</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="12">
+        <v>37.943620559999999</v>
+      </c>
+      <c r="D8" s="12">
+        <v>14.14724182</v>
+      </c>
+      <c r="E8" s="12">
+        <v>4199901</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2445070</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" t="s">
+        <v>202</v>
+      </c>
+      <c r="M8" t="s">
+        <v>183</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>20</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>7.5</v>
+      </c>
+      <c r="R8">
+        <v>4.18</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="23">
+        <v>280026</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="12">
+        <v>37.943620559999999</v>
+      </c>
+      <c r="D9" s="12">
+        <v>14.14724182</v>
+      </c>
+      <c r="E9" s="12">
+        <v>4199901</v>
+      </c>
+      <c r="F9" s="12">
+        <v>2445070</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" t="s">
+        <v>182</v>
+      </c>
+      <c r="M9" t="s">
+        <v>183</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>2.8</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="11">
+        <v>278849</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="19">
+        <v>37.989339999999999</v>
+      </c>
+      <c r="D10" s="19">
+        <v>14.193776</v>
+      </c>
+      <c r="E10" s="18">
+        <v>4204946</v>
+      </c>
+      <c r="F10" s="18">
+        <v>2449209</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="L10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M10" t="s">
+        <v>183</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>32.75</v>
+      </c>
+      <c r="R10">
+        <v>7.76</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="11">
+        <v>282679</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="12">
+        <v>37.853526049999999</v>
+      </c>
+      <c r="D11" s="12">
+        <v>14.14517684</v>
+      </c>
+      <c r="E11" s="12">
+        <v>4189906</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2444797</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>203</v>
+      </c>
+      <c r="K11" t="s">
+        <v>206</v>
+      </c>
+      <c r="L11" t="s">
+        <v>182</v>
+      </c>
+      <c r="M11" t="s">
+        <v>183</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="R11">
+        <v>12.79</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunta scheda "Valori medi x candini" dove ci sono i dati da aatribuire alle singole specie
</commit_message>
<xml_diff>
--- a/docs/Punti_INFC_rilievi.xlsx
+++ b/docs/Punti_INFC_rilievi.xlsx
@@ -4,27 +4,28 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6456" yWindow="180" windowWidth="3156" windowHeight="7092" activeTab="3"/>
+    <workbookView xWindow="6456" yWindow="180" windowWidth="3156" windowHeight="7092"/>
   </bookViews>
   <sheets>
-    <sheet name="PUNTI" sheetId="1" r:id="rId1"/>
-    <sheet name="LEGENDA" sheetId="2" r:id="rId2"/>
-    <sheet name="ALBERI" sheetId="3" r:id="rId3"/>
-    <sheet name="Medie_per_specie" sheetId="6" r:id="rId4"/>
-    <sheet name="Foglio1" sheetId="4" r:id="rId5"/>
+    <sheet name="Valori_medi_x_candini" sheetId="7" r:id="rId1"/>
+    <sheet name="PUNTI" sheetId="1" r:id="rId2"/>
+    <sheet name="LEGENDA" sheetId="2" r:id="rId3"/>
+    <sheet name="ALBERI" sheetId="3" r:id="rId4"/>
+    <sheet name="Medie generiche" sheetId="6" r:id="rId5"/>
+    <sheet name="Dati_aree_di saggio_validi" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="input278849" localSheetId="4">Foglio1!$C$14:$U$17</definedName>
-    <definedName name="input280026" localSheetId="4">Foglio1!$D$13:$V$14</definedName>
-    <definedName name="input281673" localSheetId="4">Foglio1!$G$5:$W$12</definedName>
-    <definedName name="input282422" localSheetId="4">Foglio1!$G$12:$W$12</definedName>
-    <definedName name="input282679" localSheetId="4">Foglio1!$B$13:$T$16</definedName>
-    <definedName name="input282921" localSheetId="4">Foglio1!$D$13:$V$14</definedName>
-    <definedName name="input282928" localSheetId="4">Foglio1!$G$1:$W$2</definedName>
+    <definedName name="input278849" localSheetId="5">'Dati_aree_di saggio_validi'!$C$14:$U$17</definedName>
+    <definedName name="input280026" localSheetId="5">'Dati_aree_di saggio_validi'!$D$13:$V$14</definedName>
+    <definedName name="input281673" localSheetId="5">'Dati_aree_di saggio_validi'!$G$5:$W$12</definedName>
+    <definedName name="input282422" localSheetId="5">'Dati_aree_di saggio_validi'!$G$12:$W$12</definedName>
+    <definedName name="input282679" localSheetId="5">'Dati_aree_di saggio_validi'!$B$13:$T$16</definedName>
+    <definedName name="input282921" localSheetId="5">'Dati_aree_di saggio_validi'!$D$13:$V$14</definedName>
+    <definedName name="input282928" localSheetId="5">'Dati_aree_di saggio_validi'!$G$1:$W$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId6"/>
+    <pivotCache cacheId="14" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -224,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="215">
   <si>
     <t>IDPUNTO</t>
   </si>
@@ -865,7 +866,10 @@
     <t>Etichette di riga</t>
   </si>
   <si>
-    <t>Totale complessivo</t>
+    <t>Y_planted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> N</t>
   </si>
 </sst>
 </file>
@@ -876,7 +880,7 @@
     <numFmt numFmtId="168" formatCode="0.00000000"/>
     <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -942,8 +946,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -980,8 +992,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -989,11 +1019,214 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -1043,142 +1276,45 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.000"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="170" formatCode="0.000"/>
     </dxf>
@@ -1202,9 +1338,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Alessandro Scremin" refreshedDate="41243.712199884256" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="10">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Alessandro Scremin" refreshedDate="41243.728657870372" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="10">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:R11" sheet="Foglio1"/>
+    <worksheetSource ref="A1:R11" sheet="Dati_aree_di saggio_validi"/>
   </cacheSource>
   <cacheFields count="18">
     <cacheField name="IDPUNTO" numFmtId="0">
@@ -1232,7 +1368,7 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
     </cacheField>
     <cacheField name="Age" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="100"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="10" maxValue="100"/>
     </cacheField>
     <cacheField name="Species" numFmtId="0">
       <sharedItems count="4">
@@ -1246,15 +1382,10 @@
       <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="7"/>
     </cacheField>
     <cacheField name="Phenology" numFmtId="0">
-      <sharedItems count="2">
-        <s v="D"/>
-        <s v="E"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Management" numFmtId="0">
-      <sharedItems count="1">
-        <s v="T"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Lai" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
@@ -1289,8 +1420,8 @@
     <n v="100"/>
     <x v="0"/>
     <n v="2"/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="D"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="10"/>
     <n v="0"/>
@@ -1309,8 +1440,8 @@
     <n v="10"/>
     <x v="0"/>
     <n v="2"/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="D"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="7"/>
     <n v="0"/>
@@ -1329,8 +1460,8 @@
     <n v="10"/>
     <x v="1"/>
     <n v="6"/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="D"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="12"/>
     <n v="0"/>
@@ -1346,11 +1477,11 @@
     <n v="2436827"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
+    <m/>
     <x v="1"/>
     <n v="6"/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="D"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="23"/>
     <n v="0"/>
@@ -1366,11 +1497,11 @@
     <n v="2436827"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
+    <m/>
     <x v="2"/>
     <n v="7"/>
-    <x v="1"/>
-    <x v="0"/>
+    <s v="E"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="5"/>
     <n v="0"/>
@@ -1389,8 +1520,8 @@
     <n v="20"/>
     <x v="0"/>
     <s v="2 e 7"/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="D"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="130"/>
     <n v="0"/>
@@ -1409,8 +1540,8 @@
     <n v="20"/>
     <x v="2"/>
     <m/>
-    <x v="1"/>
-    <x v="0"/>
+    <s v="E"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="20"/>
     <n v="0"/>
@@ -1429,8 +1560,8 @@
     <n v="20"/>
     <x v="1"/>
     <m/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="D"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="2"/>
     <n v="0"/>
@@ -1446,11 +1577,11 @@
     <n v="2449209"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
+    <m/>
     <x v="2"/>
     <m/>
-    <x v="1"/>
-    <x v="0"/>
+    <s v="E"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="7"/>
     <n v="0"/>
@@ -1469,8 +1600,8 @@
     <n v="25"/>
     <x v="3"/>
     <s v="1 e 6 e 7"/>
-    <x v="0"/>
-    <x v="0"/>
+    <s v="D"/>
+    <s v="T"/>
     <n v="0"/>
     <n v="5"/>
     <n v="0"/>
@@ -1481,8 +1612,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:E17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1503,69 +1634,29 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
-  <rowFields count="3">
+  <rowFields count="1">
     <field x="9"/>
-    <field x="11"/>
-    <field x="12"/>
   </rowFields>
-  <rowItems count="13">
+  <rowItems count="4">
     <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
     <i>
       <x v="2"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
     <i>
       <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -1591,8 +1682,8 @@
     <dataField name="Media di Age" fld="8" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Media di N" fld="14" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="8">
-    <format dxfId="36">
+  <formats count="4">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="1">
@@ -1601,19 +1692,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="9" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="1">
@@ -1622,19 +1701,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="11" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="40">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="1">
@@ -1643,35 +1710,11 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="9" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="11" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="42">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="1">
             <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="43">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="9" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="11" count="1">
-            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -1994,11 +2037,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1">
+      <c r="A1" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1">
+      <c r="A2" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="35">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C2" s="36">
+        <v>12.79</v>
+      </c>
+      <c r="D2" s="37">
+        <v>1981</v>
+      </c>
+      <c r="E2" s="38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1">
+      <c r="A3" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="39">
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C3" s="40">
+        <v>12.426666666666668</v>
+      </c>
+      <c r="D3" s="41">
+        <v>1962.6666666666667</v>
+      </c>
+      <c r="E3" s="42">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1">
+      <c r="A4" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="39">
+        <v>12.386666666666665</v>
+      </c>
+      <c r="C4" s="40">
+        <v>7.04</v>
+      </c>
+      <c r="D4" s="41">
+        <v>1991</v>
+      </c>
+      <c r="E4" s="42">
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1">
+      <c r="A5" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="43">
+        <v>18.473333333333333</v>
+      </c>
+      <c r="C5" s="44">
+        <v>7</v>
+      </c>
+      <c r="D5" s="45">
+        <v>1986</v>
+      </c>
+      <c r="E5" s="46">
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10:F11"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2445,11 +2594,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -3190,7 +3339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L186"/>
   <sheetViews>
@@ -7904,21 +8053,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:E17"/>
+  <dimension ref="A3:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5">
@@ -7944,224 +8093,71 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="26">
         <v>18.329999999999998</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="26">
         <v>12.79</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="26">
         <v>25</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="26">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" s="29">
-        <v>18.329999999999998</v>
-      </c>
-      <c r="C6" s="29">
-        <v>12.79</v>
-      </c>
-      <c r="D6" s="29">
-        <v>25</v>
-      </c>
-      <c r="E6" s="29">
-        <v>5</v>
+      <c r="A6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="26">
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C6" s="26">
+        <v>12.426666666666668</v>
+      </c>
+      <c r="D6" s="26">
+        <v>43.333333333333336</v>
+      </c>
+      <c r="E6" s="26">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B7" s="25">
-        <v>18.329999999999998</v>
-      </c>
-      <c r="C7" s="25">
-        <v>12.79</v>
-      </c>
-      <c r="D7" s="25">
-        <v>25</v>
-      </c>
-      <c r="E7" s="25">
-        <v>5</v>
+      <c r="A7" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="26">
+        <v>12.386666666666665</v>
+      </c>
+      <c r="C7" s="26">
+        <v>7.04</v>
+      </c>
+      <c r="D7" s="26">
+        <v>15</v>
+      </c>
+      <c r="E7" s="26">
+        <v>12.333333333333334</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="29">
-        <v>26.696666666666669</v>
-      </c>
-      <c r="C8" s="29">
-        <v>12.426666666666668</v>
-      </c>
-      <c r="D8" s="29">
-        <v>43.333333333333336</v>
-      </c>
-      <c r="E8" s="29">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="29">
-        <v>26.696666666666669</v>
-      </c>
-      <c r="C9" s="29">
-        <v>12.426666666666668</v>
-      </c>
-      <c r="D9" s="29">
-        <v>43.333333333333336</v>
-      </c>
-      <c r="E9" s="29">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B10" s="25">
-        <v>26.696666666666669</v>
-      </c>
-      <c r="C10" s="25">
-        <v>12.426666666666668</v>
-      </c>
-      <c r="D10" s="25">
-        <v>43.333333333333336</v>
-      </c>
-      <c r="E10" s="25">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11" s="29">
-        <v>12.386666666666665</v>
-      </c>
-      <c r="C11" s="29">
-        <v>7.04</v>
-      </c>
-      <c r="D11" s="29">
-        <v>10</v>
-      </c>
-      <c r="E11" s="29">
-        <v>12.333333333333334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="29">
-        <v>12.386666666666665</v>
-      </c>
-      <c r="C12" s="29">
-        <v>7.04</v>
-      </c>
-      <c r="D12" s="29">
-        <v>10</v>
-      </c>
-      <c r="E12" s="29">
-        <v>12.333333333333334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B13" s="25">
-        <v>12.386666666666665</v>
-      </c>
-      <c r="C13" s="25">
-        <v>7.04</v>
-      </c>
-      <c r="D13" s="25">
-        <v>10</v>
-      </c>
-      <c r="E13" s="25">
-        <v>12.333333333333334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B8" s="26">
         <v>18.473333333333333</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C8" s="26">
         <v>7</v>
       </c>
-      <c r="D14" s="29">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="E14" s="29">
+      <c r="D8" s="26">
+        <v>20</v>
+      </c>
+      <c r="E8" s="26">
         <v>10.666666666666666</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="B15" s="29">
-        <v>18.473333333333333</v>
-      </c>
-      <c r="C15" s="29">
-        <v>7</v>
-      </c>
-      <c r="D15" s="29">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="E15" s="29">
-        <v>10.666666666666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="25">
-        <v>18.473333333333333</v>
-      </c>
-      <c r="C16" s="25">
-        <v>7</v>
-      </c>
-      <c r="D16" s="25">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="E16" s="25">
-        <v>10.666666666666666</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="25">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="C17" s="25">
-        <v>9.2189999999999976</v>
-      </c>
-      <c r="D17" s="25">
-        <v>20.5</v>
-      </c>
-      <c r="E17" s="25">
-        <v>22.1</v>
       </c>
     </row>
   </sheetData>
@@ -8169,19 +8165,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.88671875" customWidth="1"/>
     <col min="7" max="8" width="2" bestFit="1" customWidth="1"/>
@@ -8511,9 +8507,6 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
       <c r="J5" s="3" t="s">
         <v>200</v>
       </c>
@@ -8582,9 +8575,6 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6" s="3" t="s">
         <v>201</v>
       </c>
@@ -8862,9 +8852,6 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
       <c r="J10" s="3" t="s">
         <v>201</v>
       </c>
@@ -8974,6 +8961,180 @@
       </c>
       <c r="W11">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="26">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C15" s="26">
+        <v>12.79</v>
+      </c>
+      <c r="D15" s="28">
+        <v>25</v>
+      </c>
+      <c r="E15" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="26">
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C16" s="26">
+        <v>12.426666666666668</v>
+      </c>
+      <c r="D16" s="28">
+        <v>43.333333333333336</v>
+      </c>
+      <c r="E16" s="26">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="26">
+        <v>12.386666666666665</v>
+      </c>
+      <c r="C17" s="26">
+        <v>7.04</v>
+      </c>
+      <c r="D17" s="28">
+        <v>15</v>
+      </c>
+      <c r="E17" s="26">
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="26">
+        <v>18.473333333333333</v>
+      </c>
+      <c r="C18" s="26">
+        <v>7</v>
+      </c>
+      <c r="D18" s="28">
+        <v>20</v>
+      </c>
+      <c r="E18" s="26">
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" s="26">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C21" s="26">
+        <v>12.79</v>
+      </c>
+      <c r="D21" s="28">
+        <f>2006 - D15</f>
+        <v>1981</v>
+      </c>
+      <c r="E21" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="26">
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C22" s="26">
+        <v>12.426666666666668</v>
+      </c>
+      <c r="D22" s="28">
+        <f t="shared" ref="D22:D24" si="0">2006 - D16</f>
+        <v>1962.6666666666667</v>
+      </c>
+      <c r="E22" s="26">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="26">
+        <v>12.386666666666665</v>
+      </c>
+      <c r="C23" s="26">
+        <v>7.04</v>
+      </c>
+      <c r="D23" s="28">
+        <f t="shared" si="0"/>
+        <v>1991</v>
+      </c>
+      <c r="E23" s="26">
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="26">
+        <v>18.473333333333333</v>
+      </c>
+      <c r="C24" s="26">
+        <v>7</v>
+      </c>
+      <c r="D24" s="28">
+        <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+      <c r="E24" s="26">
+        <v>10.666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>